<commit_message>
Criei o desafio 14
</commit_message>
<xml_diff>
--- a/tabelas.xlsx
+++ b/tabelas.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\paulo\OneDrive\Desktop\outros\Curso de HTML5 e CSS3\html-css\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C93FAAB3-AF65-4883-9A81-1998438D3ADB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{345247F0-F8D9-4994-9CA3-E62B54616F73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="10545" activeTab="2" xr2:uid="{522E283F-5B04-4478-A8C8-2ADB92F439A0}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="10545" activeTab="3" xr2:uid="{522E283F-5B04-4478-A8C8-2ADB92F439A0}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
     <sheet name="Planilha2" sheetId="2" r:id="rId2"/>
     <sheet name="Planilha3" sheetId="3" r:id="rId3"/>
+    <sheet name="Planilha4" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="59">
   <si>
     <t>A</t>
   </si>
@@ -153,13 +154,64 @@
   </si>
   <si>
     <t>Toy Story</t>
+  </si>
+  <si>
+    <t>Área</t>
+  </si>
+  <si>
+    <t>Disciplinas</t>
+  </si>
+  <si>
+    <t>Notas</t>
+  </si>
+  <si>
+    <t>Nota 1</t>
+  </si>
+  <si>
+    <t>Nota 2</t>
+  </si>
+  <si>
+    <t>0.0</t>
+  </si>
+  <si>
+    <t>Matemática</t>
+  </si>
+  <si>
+    <t>Física</t>
+  </si>
+  <si>
+    <t>Química</t>
+  </si>
+  <si>
+    <t>Biologia</t>
+  </si>
+  <si>
+    <t>Média de Exatas</t>
+  </si>
+  <si>
+    <t>Exatas</t>
+  </si>
+  <si>
+    <t>Média</t>
+  </si>
+  <si>
+    <t>Humanas</t>
+  </si>
+  <si>
+    <t>História</t>
+  </si>
+  <si>
+    <t>Geografia</t>
+  </si>
+  <si>
+    <t>Média de Humanas</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -187,8 +239,34 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -198,6 +276,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFF8F9FA"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.499984740745262"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -292,21 +376,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -315,6 +399,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -327,28 +415,49 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -679,13 +788,13 @@
       <c r="A1" s="7">
         <v>1</v>
       </c>
-      <c r="B1" s="8">
+      <c r="B1" s="6">
         <v>2</v>
       </c>
-      <c r="C1" s="6">
+      <c r="C1" s="10">
         <v>3</v>
       </c>
-      <c r="D1" s="8">
+      <c r="D1" s="6">
         <v>4</v>
       </c>
     </row>
@@ -693,45 +802,45 @@
       <c r="A2" s="7">
         <v>5</v>
       </c>
-      <c r="B2" s="8">
+      <c r="B2" s="6">
         <v>6</v>
       </c>
-      <c r="C2" s="6"/>
-      <c r="D2" s="8">
+      <c r="C2" s="10"/>
+      <c r="D2" s="6">
         <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="9">
+      <c r="A3" s="11">
         <v>8</v>
       </c>
-      <c r="B3" s="10"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="8">
+      <c r="B3" s="12"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="6">
         <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="12">
+      <c r="A4" s="16">
         <v>10</v>
       </c>
-      <c r="B4" s="13">
+      <c r="B4" s="14">
         <v>11</v>
       </c>
-      <c r="C4" s="14"/>
-      <c r="D4" s="8">
+      <c r="C4" s="15"/>
+      <c r="D4" s="6">
         <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="15"/>
-      <c r="B5" s="8">
+      <c r="A5" s="17"/>
+      <c r="B5" s="6">
         <v>13</v>
       </c>
-      <c r="C5" s="8">
+      <c r="C5" s="6">
         <v>14</v>
       </c>
-      <c r="D5" s="8">
+      <c r="D5" s="6">
         <v>15</v>
       </c>
     </row>
@@ -830,65 +939,65 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6" t="s">
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="6"/>
+      <c r="E2" s="10"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="6"/>
-      <c r="B3" s="8" t="s">
+      <c r="A3" s="10"/>
+      <c r="B3" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="6"/>
+      <c r="E3" s="10"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="6"/>
-      <c r="B4" s="8" t="s">
+      <c r="A4" s="10"/>
+      <c r="B4" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="6"/>
+      <c r="E4" s="10"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="6"/>
-      <c r="B5" s="6" t="s">
+      <c r="A5" s="10"/>
+      <c r="B5" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -905,7 +1014,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0513C1A-52EA-494C-9719-089B70FB5D10}">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
@@ -919,62 +1028,62 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="C1" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="19" t="s">
+      <c r="C2" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="D2" s="19" t="s">
+      <c r="D2" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="E2" s="19" t="s">
+      <c r="E2" s="9" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="18"/>
-      <c r="B3" s="19" t="s">
+      <c r="B3" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="19" t="s">
+      <c r="C3" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="D3" s="19" t="s">
+      <c r="D3" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="E3" s="19" t="s">
+      <c r="E3" s="9" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="18"/>
-      <c r="B4" s="19" t="s">
+      <c r="B4" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="19" t="s">
+      <c r="C4" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="D4" s="19" t="s">
+      <c r="D4" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="E4" s="19" t="s">
+      <c r="E4" s="9" t="s">
         <v>38</v>
       </c>
     </row>
@@ -982,46 +1091,46 @@
       <c r="A5" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="19" t="s">
+      <c r="B5" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="19" t="s">
+      <c r="C5" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="D5" s="19" t="s">
+      <c r="D5" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="E5" s="19" t="s">
+      <c r="E5" s="9" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="18"/>
-      <c r="B6" s="19" t="s">
+      <c r="B6" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="19" t="s">
+      <c r="C6" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="D6" s="19" t="s">
+      <c r="D6" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="E6" s="19" t="s">
+      <c r="E6" s="9" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="18"/>
-      <c r="B7" s="19" t="s">
+      <c r="B7" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C7" s="19" t="s">
+      <c r="C7" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="D7" s="19" t="s">
+      <c r="D7" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="E7" s="19" t="s">
+      <c r="E7" s="9" t="s">
         <v>41</v>
       </c>
     </row>
@@ -1033,4 +1142,177 @@
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{933661D2-549A-4234-98AD-461685CCF5F3}">
+  <dimension ref="A1:E10"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.42578125" customWidth="1"/>
+    <col min="2" max="2" width="24" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="A1" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1" s="25" t="s">
+        <v>44</v>
+      </c>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="A2" s="24"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="26" t="s">
+        <v>45</v>
+      </c>
+      <c r="D2" s="26" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2" s="25"/>
+    </row>
+    <row r="3" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="A3" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="B3" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="C3" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="D3" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="E3" s="21" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="A4" s="23"/>
+      <c r="B4" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="C4" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="D4" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="E4" s="21" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="A5" s="23"/>
+      <c r="B5" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="C5" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="D5" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="E5" s="21" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="A6" s="23"/>
+      <c r="B6" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="C6" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="D6" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="E6" s="21" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="A7" s="27" t="s">
+        <v>52</v>
+      </c>
+      <c r="B7" s="27"/>
+      <c r="C7" s="27"/>
+      <c r="D7" s="27"/>
+      <c r="E7" s="26" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="A8" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="B8" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="C8" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="D8" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="E8" s="21" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="A9" s="23"/>
+      <c r="B9" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="C9" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="D9" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="E9" s="21" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="A10" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="B10" s="28"/>
+      <c r="C10" s="28"/>
+      <c r="D10" s="28"/>
+      <c r="E10" s="26" t="s">
+        <v>47</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="A10:D10"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="A7:D7"/>
+    <mergeCell ref="A3:A6"/>
+    <mergeCell ref="E1:E2"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>